<commit_message>
fifth presentation is added in the first version
</commit_message>
<xml_diff>
--- a/gpacalculator.xlsx
+++ b/gpacalculator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OKUL\ee_polimi_finito\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OKUL\ee_polimi_finito\thesisWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F276192-0A1C-43C4-BD79-ED76D897A4F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB2D707-1118-4062-B35D-7F147D9F30BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -401,7 +401,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,10 +424,10 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -447,10 +447,10 @@
         <v>18</v>
       </c>
       <c r="E2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H2">
         <v>7</v>
@@ -495,19 +495,19 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <f>SUM(B2*B3,C2*C3,D2*D3,E2*E3,F2*F3)/C7</f>
-        <v>25.65</v>
+        <f>SUM(B2*B3,C2*C3,D2*D3,F2*F3,E2*E3)/C7</f>
+        <v>25.85</v>
       </c>
       <c r="J6" t="s">
         <v>8</v>
       </c>
       <c r="K6">
         <f>K7*4/110</f>
-        <v>3.6745454545454543</v>
+        <v>3.7012121212121212</v>
       </c>
       <c r="M6">
-        <f>SUM(C2*C3,D2*D3,E2*E3,F2*F3)/SUM(C3,D3,E3,F3)</f>
-        <v>25.25</v>
+        <f>SUM(C2*C3,D2*D3,F2*F3,E2*E3)/SUM(C3,D3,F3,E3)</f>
+        <v>26.25</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -515,7 +515,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <f>SUM(B3,C3,D3,E3,F3)</f>
+        <f>SUM(B3,C3,D3,F3,E3)</f>
         <v>100</v>
       </c>
       <c r="J7" t="s">
@@ -523,7 +523,7 @@
       </c>
       <c r="K7">
         <f>SUM(C6*(110/30), H2)</f>
-        <v>101.05</v>
+        <v>101.78333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new figures added for the new presentation and updated gpa calculator
</commit_message>
<xml_diff>
--- a/gpacalculator.xlsx
+++ b/gpacalculator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OKUL\ee_polimi_finito\thesisWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB2D707-1118-4062-B35D-7F147D9F30BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301F9242-751B-46B6-B5C0-50EBB3181C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -401,7 +401,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated with respect to minimum 101/110L grade
</commit_message>
<xml_diff>
--- a/gpacalculator.xlsx
+++ b/gpacalculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OKUL\ee_polimi_finito\thesisWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301F9242-751B-46B6-B5C0-50EBB3181C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DBBAFF-2073-422C-B487-C7F83B5B10DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -401,7 +401,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,7 +453,7 @@
         <v>30</v>
       </c>
       <c r="H2">
-        <v>7</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -503,7 +503,7 @@
       </c>
       <c r="K6">
         <f>K7*4/110</f>
-        <v>3.7012121212121212</v>
+        <v>3.6757575757575758</v>
       </c>
       <c r="M6">
         <f>SUM(C2*C3,D2*D3,F2*F3,E2*E3)/SUM(C3,D3,F3,E3)</f>
@@ -523,7 +523,7 @@
       </c>
       <c r="K7">
         <f>SUM(C6*(110/30), H2)</f>
-        <v>101.78333333333333</v>
+        <v>101.08333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>